<commit_message>
Reto con las correciones
</commit_message>
<xml_diff>
--- a/Casos de Prueba.xlsx
+++ b/Casos de Prueba.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26216"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="535" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{620F0563-AEBD-4B83-8017-00D68D835ECB}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C436ECF0-FDAB-41FA-9387-589FB5895EEF}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Casos de Pruebas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -490,11 +490,158 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,154 +659,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1008,7 +1008,7 @@
       <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="69" t="s">
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="8" t="s">
@@ -1017,297 +1017,297 @@
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="2:9" ht="45.75" customHeight="1">
-      <c r="B3" s="40">
+      <c r="B3" s="38">
         <v>1</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="40"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="53"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="57"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="40"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="53"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="57"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="B6" s="40">
+      <c r="B6" s="38">
         <v>2</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:9">
-      <c r="B7" s="40"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="57"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="14"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="57"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="2:9" ht="15" customHeight="1">
-      <c r="B9" s="40">
+      <c r="B9" s="38">
         <v>3</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="40"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="57"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="2:9" ht="30.75" customHeight="1">
-      <c r="B11" s="14"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="57"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="27">
+      <c r="B12" s="21">
         <v>4</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="27"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="57"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="2:9" ht="33" customHeight="1">
-      <c r="B14" s="35"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="2:9" ht="33" customHeight="1">
-      <c r="B15" s="27">
+      <c r="B15" s="21">
         <v>5</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="33" customHeight="1">
-      <c r="B16" s="27"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="26"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" spans="2:8" ht="0.75" customHeight="1">
-      <c r="B17" s="27"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="1"/>
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="2:8" ht="33" hidden="1" customHeight="1">
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="1"/>
       <c r="H18" s="11"/>
     </row>
     <row r="19" spans="2:8" ht="33" customHeight="1">
-      <c r="B19" s="27">
+      <c r="B19" s="21">
         <v>6</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B20" s="27"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="67"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="63"/>
     </row>
     <row r="21" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B21" s="14">
+      <c r="B21" s="39">
         <v>7</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="66" t="s">
+      <c r="H21" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="26.25" customHeight="1">
-      <c r="B22" s="15"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="66"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="2:8" ht="9" customHeight="1">
-      <c r="B23" s="16"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="66"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="2:8" ht="35.25" customHeight="1">
-      <c r="B24" s="56">
+      <c r="B24" s="20">
         <v>6</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="12" t="s">
@@ -1322,13 +1322,13 @@
       <c r="G24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="68" t="s">
+      <c r="H24" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="45.75" customHeight="1">
-      <c r="B25" s="27"/>
-      <c r="C25" s="55"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1341,11 +1341,11 @@
       <c r="G25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="65"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="2:8" ht="47.25" customHeight="1">
-      <c r="B26" s="27"/>
-      <c r="C26" s="55"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="5" t="s">
         <v>41</v>
       </c>
@@ -1358,13 +1358,13 @@
       <c r="G26" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="64" t="s">
+      <c r="H26" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="78.75" customHeight="1">
-      <c r="B27" s="27"/>
-      <c r="C27" s="55"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="4" t="s">
         <v>43</v>
       </c>
@@ -1377,15 +1377,36 @@
       <c r="G27" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="65"/>
+      <c r="H27" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
     <mergeCell ref="H3:H5"/>
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="H9:H11"/>
@@ -1402,32 +1423,11 @@
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B24:B27"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="C21:C23"/>

</xml_diff>